<commit_message>
Annotated w/ BLAST info
</commit_message>
<xml_diff>
--- a/16S/SummerContentABX_TaxTable.xlsx
+++ b/16S/SummerContentABX_TaxTable.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7ecf4928fe261446/Documents/GitHub/Carb_CRDS/16S/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{E33A23D0-8B69-4FF2-9317-B4836DCD2ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="102" documentId="13_ncr:40009_{E33A23D0-8B69-4FF2-9317-B4836DCD2ACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{466814B4-1E4D-4D46-92E8-E40C9284BA44}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="11388"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SummerContentABX_TaxTable" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="558">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="919" uniqueCount="576">
   <si>
     <t>OTU</t>
   </si>
@@ -1694,12 +1694,66 @@
   </si>
   <si>
     <t>Lachnospiraceae_FCS020_group</t>
+  </si>
+  <si>
+    <t>Max Score</t>
+  </si>
+  <si>
+    <t>Query Cover (%)</t>
+  </si>
+  <si>
+    <t>E-value</t>
+  </si>
+  <si>
+    <t>% Identity</t>
+  </si>
+  <si>
+    <t>Morganella morganii</t>
+  </si>
+  <si>
+    <t>BLAST Match</t>
+  </si>
+  <si>
+    <t>Unclassified / thetaiotaomicron / faecis / faecichinchillae / zhangwenhongii</t>
+  </si>
+  <si>
+    <t>Uncultured</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncultured / murinus / animalis / Liglactobacillus murinus / Liglactobacillus animalis / faecis / apodemi </t>
+  </si>
+  <si>
+    <t>Uncultured / sp. CT06 / distasonis</t>
+  </si>
+  <si>
+    <t>Uncultured / Fusimonas intestini</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncultured / sartorii / Phocaeicola sartorii / </t>
+  </si>
+  <si>
+    <t>Bacteroides caecimuris</t>
+  </si>
+  <si>
+    <t>uncultured / Eubacteriales bacterium</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncultured / marseillensis / rara </t>
+  </si>
+  <si>
+    <t>Uncultured / rodentium</t>
+  </si>
+  <si>
+    <t>Uncultured / stercorirosoris / oleiciplenus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Uncultured </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1836,7 +1890,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2022,12 +2076,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="0"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2193,7 +2241,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2548,19 +2596,24 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E446"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:J446"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="33.33203125" customWidth="1"/>
+    <col min="2" max="2" width="33.28515625" customWidth="1"/>
+    <col min="6" max="6" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.5703125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2576,8 +2629,23 @@
       <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="1" t="s">
+        <v>563</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>558</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>559</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
@@ -2593,8 +2661,23 @@
       <c r="E2" s="2">
         <v>13.9039167054211</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F2" t="s">
+        <v>564</v>
+      </c>
+      <c r="G2" s="2">
+        <v>468</v>
+      </c>
+      <c r="H2" s="2">
+        <v>100</v>
+      </c>
+      <c r="I2" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J2" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>52</v>
       </c>
@@ -2610,8 +2693,23 @@
       <c r="E3" s="2">
         <v>15.1632343936318</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F3" t="s">
+        <v>565</v>
+      </c>
+      <c r="G3" s="2">
+        <v>403</v>
+      </c>
+      <c r="H3" s="2">
+        <v>99</v>
+      </c>
+      <c r="I3" s="3">
+        <v>5E-108</v>
+      </c>
+      <c r="J3" s="2">
+        <v>95.63</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>11</v>
       </c>
@@ -2627,8 +2725,23 @@
       <c r="E4" s="2">
         <v>7.6191230541105197</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F4" t="s">
+        <v>566</v>
+      </c>
+      <c r="G4" s="2">
+        <v>468</v>
+      </c>
+      <c r="H4" s="2">
+        <v>100</v>
+      </c>
+      <c r="I4" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J4" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -2644,8 +2757,23 @@
       <c r="E5" s="2">
         <v>6.2900328941207997</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F5" t="s">
+        <v>567</v>
+      </c>
+      <c r="G5" s="2">
+        <v>468</v>
+      </c>
+      <c r="H5" s="2">
+        <v>100</v>
+      </c>
+      <c r="I5" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J5" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>17</v>
       </c>
@@ -2661,246 +2789,471 @@
       <c r="E6" s="2">
         <v>3.2264779936569701</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
+      <c r="F6" t="s">
+        <v>568</v>
+      </c>
+      <c r="G6" s="2">
+        <v>468</v>
+      </c>
+      <c r="H6" s="2">
+        <v>100</v>
+      </c>
+      <c r="I6" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J6" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="3">
+      <c r="C7" s="2">
         <v>3.1850130001438899</v>
       </c>
-      <c r="D7" s="3">
+      <c r="D7" s="2">
         <v>4.2629822717114898</v>
       </c>
-      <c r="E7" s="3">
+      <c r="E7" s="2">
         <v>2.46123396212323</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
+      <c r="F7" t="s">
+        <v>569</v>
+      </c>
+      <c r="G7" s="2">
+        <v>468</v>
+      </c>
+      <c r="H7" s="2">
+        <v>100</v>
+      </c>
+      <c r="I7" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J7" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="3">
+      <c r="C8" s="2">
         <v>2.6365890712385101</v>
       </c>
-      <c r="D8" s="3">
+      <c r="D8" s="2">
         <v>2.12605027365277</v>
       </c>
-      <c r="E8" s="3">
+      <c r="E8" s="2">
         <v>1.2274756978041099</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
+      <c r="F8" t="s">
+        <v>570</v>
+      </c>
+      <c r="G8" s="2">
+        <v>462</v>
+      </c>
+      <c r="H8" s="2">
+        <v>100</v>
+      </c>
+      <c r="I8" s="3">
+        <v>7.9999999999999996E-126</v>
+      </c>
+      <c r="J8" s="2">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="3">
+      <c r="C9" s="2">
         <v>2.1989986168386699</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D9" s="2">
         <v>3.7920435393455199</v>
       </c>
-      <c r="E9" s="3">
+      <c r="E9" s="2">
         <v>2.18933735821992</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
+      <c r="F9" t="s">
+        <v>571</v>
+      </c>
+      <c r="G9" s="2">
+        <v>457</v>
+      </c>
+      <c r="H9" s="2">
+        <v>100</v>
+      </c>
+      <c r="I9" s="3">
+        <v>3.9999999999999997E-124</v>
+      </c>
+      <c r="J9" s="2">
+        <v>99.21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="C10" s="3">
+      <c r="C10" s="2">
         <v>2.1122528171183399</v>
       </c>
-      <c r="D10" s="3">
+      <c r="D10" s="2">
         <v>3.1132938937994301</v>
       </c>
-      <c r="E10" s="3">
+      <c r="E10" s="2">
         <v>1.7974610676515199</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
+      <c r="F10" t="s">
+        <v>565</v>
+      </c>
+      <c r="G10" s="2">
+        <v>339</v>
+      </c>
+      <c r="H10" s="2">
+        <v>100</v>
+      </c>
+      <c r="I10" s="3">
+        <v>9.9999999999999993E-89</v>
+      </c>
+      <c r="J10" s="2">
+        <v>90.98</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>208</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C11" s="3">
+      <c r="C11" s="2">
         <v>1.89822424183828</v>
       </c>
-      <c r="D11" s="3">
+      <c r="D11" s="2">
         <v>3.2878208310228101</v>
       </c>
-      <c r="E11" s="3">
+      <c r="E11" s="2">
         <v>1.89822424183828</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
+      <c r="F11" t="s">
+        <v>565</v>
+      </c>
+      <c r="G11" s="2">
+        <v>468</v>
+      </c>
+      <c r="H11" s="2">
+        <v>100</v>
+      </c>
+      <c r="I11" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J11" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="3">
+      <c r="C12" s="2">
         <v>1.8398611256583399</v>
       </c>
-      <c r="D12" s="3">
+      <c r="D12" s="2">
         <v>3.1549467737759298</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="2">
         <v>1.82150936911848</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
+      <c r="F12" t="s">
+        <v>572</v>
+      </c>
+      <c r="G12" s="2">
+        <v>412</v>
+      </c>
+      <c r="H12" s="2">
+        <v>100</v>
+      </c>
+      <c r="I12" s="3">
+        <v>8.0000000000000007E-111</v>
+      </c>
+      <c r="J12" s="2">
+        <v>96.05</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="3">
+      <c r="C13" s="2">
         <v>1.77407891615546</v>
       </c>
-      <c r="D13" s="3">
+      <c r="D13" s="2">
         <v>3.0393640986688202</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="2">
         <v>1.7547776805317301</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
+      <c r="F13" t="s">
+        <v>562</v>
+      </c>
+      <c r="G13" s="2">
+        <v>568</v>
+      </c>
+      <c r="H13" s="2">
+        <v>100</v>
+      </c>
+      <c r="I13" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J13" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C14" s="3">
+      <c r="C14" s="2">
         <v>1.6667785712196199</v>
       </c>
-      <c r="D14" s="3">
+      <c r="D14" s="2">
         <v>1.5517361827596099</v>
       </c>
-      <c r="E14" s="3">
+      <c r="E14" s="2">
         <v>0.89589530282754504</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
+      <c r="F14" t="s">
+        <v>573</v>
+      </c>
+      <c r="G14" s="2">
+        <v>457</v>
+      </c>
+      <c r="H14" s="2">
+        <v>100</v>
+      </c>
+      <c r="I14" s="3">
+        <v>3.9999999999999997E-124</v>
+      </c>
+      <c r="J14" s="2">
+        <v>99.21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>113</v>
       </c>
-      <c r="C15" s="3">
+      <c r="C15" s="2">
         <v>1.3344152916779399</v>
       </c>
-      <c r="D15" s="3">
+      <c r="D15" s="2">
         <v>2.31127508358303</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E15" s="2">
         <v>1.3344152916779399</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
+      <c r="F15" t="s">
+        <v>565</v>
+      </c>
+      <c r="G15" s="2">
+        <v>468</v>
+      </c>
+      <c r="H15" s="2">
+        <v>100</v>
+      </c>
+      <c r="I15" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J15" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="3">
+      <c r="C16" s="2">
         <v>1.2446269408656401</v>
       </c>
-      <c r="D16" s="3">
+      <c r="D16" s="2">
         <v>1.19388810835799</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="2">
         <v>0.68929162074277806</v>
       </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
+      <c r="F16" t="s">
+        <v>565</v>
+      </c>
+      <c r="G16" s="2">
+        <v>435</v>
+      </c>
+      <c r="H16" s="2">
+        <v>100</v>
+      </c>
+      <c r="I16" s="3">
+        <v>2.0000000000000001E-117</v>
+      </c>
+      <c r="J16" s="2">
+        <v>97.63</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="B17" s="3" t="s">
+      <c r="B17" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="3">
+      <c r="C17" s="2">
         <v>1.2140074565219401</v>
       </c>
-      <c r="D17" s="3">
+      <c r="D17" s="2">
         <v>2.0718082618581399</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E17" s="2">
         <v>1.1961590576930901</v>
       </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
+      <c r="F17" t="s">
+        <v>565</v>
+      </c>
+      <c r="G17" s="2">
+        <v>468</v>
+      </c>
+      <c r="H17" s="2">
+        <v>100</v>
+      </c>
+      <c r="I17" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J17" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C18" s="3">
+      <c r="C18" s="2">
         <v>1.17295643854308</v>
       </c>
-      <c r="D18" s="3">
+      <c r="D18" s="2">
         <v>1.9982214769081601</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E18" s="2">
         <v>1.15367370759342</v>
       </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
+      <c r="F18" t="s">
+        <v>574</v>
+      </c>
+      <c r="G18" s="2">
+        <v>468</v>
+      </c>
+      <c r="H18" s="2">
+        <v>100</v>
+      </c>
+      <c r="I18" s="3">
+        <v>2.0000000000000001E-127</v>
+      </c>
+      <c r="J18" s="2">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" s="2" t="s">
         <v>259</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="2" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="3">
+      <c r="C19" s="2">
         <v>1.05385284733636</v>
       </c>
-      <c r="D19" s="3">
+      <c r="D19" s="2">
         <v>1.82532667528771</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E19" s="2">
         <v>1.05385284733636</v>
       </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
+      <c r="F19" t="s">
+        <v>565</v>
+      </c>
+      <c r="G19" s="2">
+        <v>379</v>
+      </c>
+      <c r="H19" s="2">
+        <v>100</v>
+      </c>
+      <c r="I19" s="3">
+        <v>8.0000000000000004E-101</v>
+      </c>
+      <c r="J19" s="2">
+        <v>63.73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="C20" s="3">
+      <c r="C20" s="2">
         <v>1.01171932947634</v>
       </c>
-      <c r="D20" s="3">
+      <c r="D20" s="2">
         <v>1.7523492816525399</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E20" s="2">
         <v>1.01171932947634</v>
       </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F20" t="s">
+        <v>575</v>
+      </c>
+      <c r="G20" s="2">
+        <v>462</v>
+      </c>
+      <c r="H20" s="2">
+        <v>100</v>
+      </c>
+      <c r="I20" s="3">
+        <v>7.9999999999999996E-126</v>
+      </c>
+      <c r="J20" s="2">
+        <v>99.6</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>63</v>
       </c>
@@ -2917,7 +3270,7 @@
         <v>0.81315886750708199</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>143</v>
       </c>
@@ -2934,7 +3287,7 @@
         <v>0.91527280930742205</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>87</v>
       </c>
@@ -2951,7 +3304,7 @@
         <v>0.80569789551709703</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>141</v>
       </c>
@@ -2968,7 +3321,7 @@
         <v>0.73329838000154501</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>51</v>
       </c>
@@ -2985,7 +3338,7 @@
         <v>0.61014563214644602</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>45</v>
       </c>
@@ -3002,7 +3355,7 @@
         <v>0.56103626122626704</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>47</v>
       </c>
@@ -3019,7 +3372,7 @@
         <v>0.33693833030804698</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>282</v>
       </c>
@@ -3036,7 +3389,7 @@
         <v>0.67034064907022495</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>36</v>
       </c>
@@ -3053,7 +3406,7 @@
         <v>0.59159481969110095</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>233</v>
       </c>
@@ -3070,7 +3423,7 @@
         <v>0.56642361146044995</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>67</v>
       </c>
@@ -3087,7 +3440,7 @@
         <v>0.53404539385847805</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>55</v>
       </c>
@@ -3104,7 +3457,7 @@
         <v>0.52195169526333696</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>153</v>
       </c>
@@ -3121,7 +3474,7 @@
         <v>0.44680693951384098</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>43</v>
       </c>
@@ -3138,7 +3491,7 @@
         <v>0.45763640465371103</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>40</v>
       </c>
@@ -3155,7 +3508,7 @@
         <v>0.30252787307262802</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>145</v>
       </c>
@@ -3172,7 +3525,7 @@
         <v>0.41251732250475398</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>182</v>
       </c>
@@ -3189,7 +3542,7 @@
         <v>0.37976561341047299</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>269</v>
       </c>
@@ -3206,7 +3559,7 @@
         <v>0.35907110510705198</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>110</v>
       </c>
@@ -3223,7 +3576,7 @@
         <v>0.29917341232774702</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>156</v>
       </c>
@@ -3240,7 +3593,7 @@
         <v>0.35306334371754899</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>319</v>
       </c>
@@ -3257,7 +3610,7 @@
         <v>0.34161590769924899</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>112</v>
       </c>
@@ -3274,7 +3627,7 @@
         <v>0.34119566829847198</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>117</v>
       </c>
@@ -3291,7 +3644,7 @@
         <v>0.324616153100653</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>306</v>
       </c>
@@ -3308,7 +3661,7 @@
         <v>0.32932799287939502</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>70</v>
       </c>
@@ -3325,7 +3678,7 @@
         <v>0.27388431643581501</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>381</v>
       </c>
@@ -3342,7 +3695,7 @@
         <v>0.322279158206839</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>149</v>
       </c>
@@ -3359,7 +3712,7 @@
         <v>0.29669188547693198</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>60</v>
       </c>
@@ -3376,7 +3729,7 @@
         <v>0.27592345349354702</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>222</v>
       </c>
@@ -3393,7 +3746,7 @@
         <v>0.26406857072302098</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>178</v>
       </c>
@@ -3410,7 +3763,7 @@
         <v>0.25204097608491099</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>28</v>
       </c>
@@ -3427,7 +3780,7 @@
         <v>0.15603839433202499</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>180</v>
       </c>
@@ -3444,7 +3797,7 @@
         <v>0.21772941903951501</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>109</v>
       </c>
@@ -3461,7 +3814,7 @@
         <v>0.21364306484345999</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>147</v>
       </c>
@@ -3478,7 +3831,7 @@
         <v>0.20905847437459699</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>378</v>
       </c>
@@ -3495,7 +3848,7 @@
         <v>0.212704244416514</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>7</v>
       </c>
@@ -3512,7 +3865,7 @@
         <v>8.7564652562259704E-2</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>192</v>
       </c>
@@ -3529,7 +3882,7 @@
         <v>0.177854121708341</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>161</v>
       </c>
@@ -3546,7 +3899,7 @@
         <v>0.18398410499596199</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>437</v>
       </c>
@@ -3563,7 +3916,7 @@
         <v>0.19014470334203501</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>391</v>
       </c>
@@ -3580,7 +3933,7 @@
         <v>0.15056457835036699</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>102</v>
       </c>
@@ -3597,7 +3950,7 @@
         <v>6.2100115134820097E-2</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>57</v>
       </c>
@@ -3614,7 +3967,7 @@
         <v>9.2252555502574204E-2</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>202</v>
       </c>
@@ -3631,7 +3984,7 @@
         <v>0.14263096811302101</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>101</v>
       </c>
@@ -3648,7 +4001,7 @@
         <v>5.2058983734816197E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>217</v>
       </c>
@@ -3665,7 +4018,7 @@
         <v>0.148398751178311</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>82</v>
       </c>
@@ -3682,7 +4035,7 @@
         <v>9.1098304443647096E-2</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>188</v>
       </c>
@@ -3699,7 +4052,7 @@
         <v>0.13213995623984101</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>74</v>
       </c>
@@ -3716,7 +4069,7 @@
         <v>0.136478267319389</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>134</v>
       </c>
@@ -3733,7 +4086,7 @@
         <v>0.12610165496471101</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>167</v>
       </c>
@@ -3750,7 +4103,7 @@
         <v>0.13054442960984999</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>370</v>
       </c>
@@ -3767,7 +4120,7 @@
         <v>0.127577510755081</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>114</v>
       </c>
@@ -3784,7 +4137,7 @@
         <v>0.11712789126956</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>209</v>
       </c>
@@ -3801,7 +4154,7 @@
         <v>8.76096981518521E-2</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>358</v>
       </c>
@@ -3818,7 +4171,7 @@
         <v>0.122466080118599</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>252</v>
       </c>
@@ -3835,7 +4188,7 @@
         <v>0.10673177786700599</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>191</v>
       </c>
@@ -3852,7 +4205,7 @@
         <v>6.83003857931994E-2</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>423</v>
       </c>
@@ -3869,7 +4222,7 @@
         <v>0.10535431885785999</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>183</v>
       </c>
@@ -3886,7 +4239,7 @@
         <v>0.10812198879929</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>181</v>
       </c>
@@ -3903,7 +4256,7 @@
         <v>5.9573718846904197E-2</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>26</v>
       </c>
@@ -3920,7 +4273,7 @@
         <v>0.10662097521428</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>131</v>
       </c>
@@ -3937,7 +4290,7 @@
         <v>0.10977599762646501</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>253</v>
       </c>
@@ -3954,7 +4307,7 @@
         <v>0.106809078771696</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>66</v>
       </c>
@@ -3971,7 +4324,7 @@
         <v>5.2102058575119702E-2</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>124</v>
       </c>
@@ -3988,7 +4341,7 @@
         <v>9.9303075315900893E-2</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -4005,7 +4358,7 @@
         <v>4.6570945157139998E-2</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>198</v>
       </c>
@@ -4022,7 +4375,7 @@
         <v>0.103129330626188</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>250</v>
       </c>
@@ -4039,7 +4392,7 @@
         <v>0.103129330626188</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>276</v>
       </c>
@@ -4056,7 +4409,7 @@
         <v>9.36975740503945E-2</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>76</v>
       </c>
@@ -4073,7 +4426,7 @@
         <v>9.3079483627781207E-2</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>403</v>
       </c>
@@ -4090,7 +4443,7 @@
         <v>0.10087524106215701</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>139</v>
       </c>
@@ -4107,7 +4460,7 @@
         <v>1.7583871818246E-2</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>186</v>
       </c>
@@ -4124,7 +4477,7 @@
         <v>7.7437130614313093E-2</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>154</v>
       </c>
@@ -4141,7 +4494,7 @@
         <v>9.0406181148314002E-2</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>174</v>
       </c>
@@ -4158,7 +4511,7 @@
         <v>9.4941403352618303E-2</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>249</v>
       </c>
@@ -4175,7 +4528,7 @@
         <v>9.4941403352618303E-2</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>184</v>
       </c>
@@ -4192,7 +4545,7 @@
         <v>9.0238164297914897E-2</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>246</v>
       </c>
@@ -4209,7 +4562,7 @@
         <v>9.0238164297914897E-2</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>295</v>
       </c>
@@ -4226,7 +4579,7 @@
         <v>7.5736884548544506E-2</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>361</v>
       </c>
@@ -4243,7 +4596,7 @@
         <v>8.9007565643079697E-2</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>121</v>
       </c>
@@ -4260,7 +4613,7 @@
         <v>5.1392832463703603E-2</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>331</v>
       </c>
@@ -4277,7 +4630,7 @@
         <v>7.7276899158515794E-2</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>421</v>
       </c>
@@ -4294,7 +4647,7 @@
         <v>8.0569789551709695E-2</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>338</v>
       </c>
@@ -4311,7 +4664,7 @@
         <v>7.5681939937049303E-2</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>280</v>
       </c>
@@ -4328,7 +4681,7 @@
         <v>5.3478348885976502E-2</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>163</v>
       </c>
@@ -4345,7 +4698,7 @@
         <v>7.7346997969641298E-2</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>230</v>
       </c>
@@ -4362,7 +4715,7 @@
         <v>7.2716847750376304E-2</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>92</v>
       </c>
@@ -4379,7 +4732,7 @@
         <v>7.7139890224002403E-2</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>312</v>
       </c>
@@ -4396,7 +4749,7 @@
         <v>7.7139890224002403E-2</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>332</v>
       </c>
@@ -4413,7 +4766,7 @@
         <v>5.5327959267801499E-2</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>171</v>
       </c>
@@ -4430,7 +4783,7 @@
         <v>7.4172971369233107E-2</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>279</v>
       </c>
@@ -4447,7 +4800,7 @@
         <v>7.4172971369233107E-2</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>21</v>
       </c>
@@ -4464,7 +4817,7 @@
         <v>6.3144099514910998E-2</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>236</v>
       </c>
@@ -4481,7 +4834,7 @@
         <v>5.8322203869842097E-2</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>375</v>
       </c>
@@ -4498,7 +4851,7 @@
         <v>7.0901414805504506E-2</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>99</v>
       </c>
@@ -4515,7 +4868,7 @@
         <v>6.6227069081472495E-2</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>289</v>
       </c>
@@ -4532,7 +4885,7 @@
         <v>3.5321172900371602E-2</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>104</v>
       </c>
@@ -4549,7 +4902,7 @@
         <v>3.4478826884849399E-2</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>151</v>
       </c>
@@ -4566,7 +4919,7 @@
         <v>3.4478826884849399E-2</v>
       </c>
     </row>
-    <row r="119" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>265</v>
       </c>
@@ -4583,7 +4936,7 @@
         <v>6.8239133659694404E-2</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>158</v>
       </c>
@@ -4600,7 +4953,7 @@
         <v>6.3006894674465103E-2</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>177</v>
       </c>
@@ -4617,7 +4970,7 @@
         <v>5.6224576469766599E-2</v>
       </c>
     </row>
-    <row r="122" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>136</v>
       </c>
@@ -4634,7 +4987,7 @@
         <v>3.8560515489629001E-2</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>226</v>
       </c>
@@ -4651,7 +5004,7 @@
         <v>5.2447804928810501E-2</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>89</v>
       </c>
@@ -4668,7 +5021,7 @@
         <v>3.0766672234427601E-2</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>142</v>
       </c>
@@ -4685,7 +5038,7 @@
         <v>3.3779836242875401E-2</v>
       </c>
     </row>
-    <row r="126" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>150</v>
       </c>
@@ -4702,7 +5055,7 @@
         <v>5.7894194372633601E-2</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>175</v>
       </c>
@@ -4719,7 +5072,7 @@
         <v>2.56696874157494E-2</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>328</v>
       </c>
@@ -4736,7 +5089,7 @@
         <v>5.1801288286729898E-2</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>108</v>
       </c>
@@ -4753,7 +5106,7 @@
         <v>5.9338377095386398E-2</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>390</v>
       </c>
@@ -4770,7 +5123,7 @@
         <v>5.9338377095386398E-2</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>313</v>
       </c>
@@ -4787,7 +5140,7 @@
         <v>5.4787456895162602E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>97</v>
       </c>
@@ -4804,7 +5157,7 @@
         <v>4.0750710139330099E-2</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>410</v>
       </c>
@@ -4821,7 +5174,7 @@
         <v>4.9004071249418302E-2</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>64</v>
       </c>
@@ -4838,7 +5191,7 @@
         <v>5.3404539385847799E-2</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>229</v>
       </c>
@@ -4855,7 +5208,7 @@
         <v>4.1656684871190501E-2</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>146</v>
       </c>
@@ -4872,7 +5225,7 @@
         <v>2.7961165233651102E-2</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>195</v>
       </c>
@@ -4889,7 +5242,7 @@
         <v>2.6130123860570599E-2</v>
       </c>
     </row>
-    <row r="138" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>120</v>
       </c>
@@ -4906,7 +5259,7 @@
         <v>4.74707016763092E-2</v>
       </c>
     </row>
-    <row r="139" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>225</v>
       </c>
@@ -4923,7 +5276,7 @@
         <v>4.74707016763092E-2</v>
       </c>
     </row>
-    <row r="140" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>337</v>
       </c>
@@ -4940,7 +5293,7 @@
         <v>4.74707016763092E-2</v>
       </c>
     </row>
-    <row r="141" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>309</v>
       </c>
@@ -4957,7 +5310,7 @@
         <v>1.02506767161103E-2</v>
       </c>
     </row>
-    <row r="142" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>190</v>
       </c>
@@ -4974,7 +5327,7 @@
         <v>2.2050913029094999E-2</v>
       </c>
     </row>
-    <row r="143" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>228</v>
       </c>
@@ -4991,7 +5344,7 @@
         <v>4.0022903420889197E-2</v>
       </c>
     </row>
-    <row r="144" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>80</v>
       </c>
@@ -5008,7 +5361,7 @@
         <v>3.6045921388247297E-2</v>
       </c>
     </row>
-    <row r="145" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>520</v>
       </c>
@@ -5025,7 +5378,7 @@
         <v>3.6074474175740001E-2</v>
       </c>
     </row>
-    <row r="146" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>218</v>
       </c>
@@ -5042,7 +5395,7 @@
         <v>4.1896290566888997E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>79</v>
       </c>
@@ -5059,7 +5412,7 @@
         <v>3.30106141390277E-2</v>
       </c>
     </row>
-    <row r="148" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>342</v>
       </c>
@@ -5076,7 +5429,7 @@
         <v>4.1536863966770497E-2</v>
       </c>
     </row>
-    <row r="149" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
         <v>441</v>
       </c>
@@ -5093,7 +5446,7 @@
         <v>4.1536863966770497E-2</v>
       </c>
     </row>
-    <row r="150" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
         <v>475</v>
       </c>
@@ -5110,7 +5463,7 @@
         <v>3.8673498984820601E-2</v>
       </c>
     </row>
-    <row r="151" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
         <v>197</v>
       </c>
@@ -5127,7 +5480,7 @@
         <v>3.8569945112001201E-2</v>
       </c>
     </row>
-    <row r="152" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
         <v>284</v>
       </c>
@@ -5144,7 +5497,7 @@
         <v>3.40642905494625E-2</v>
       </c>
     </row>
-    <row r="153" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
         <v>211</v>
       </c>
@@ -5161,7 +5514,7 @@
         <v>2.0580881740074199E-2</v>
       </c>
     </row>
-    <row r="154" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
         <v>214</v>
       </c>
@@ -5178,7 +5531,7 @@
         <v>2.2177778066820999E-2</v>
       </c>
     </row>
-    <row r="155" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
         <v>35</v>
       </c>
@@ -5195,7 +5548,7 @@
         <v>2.35276226767718E-2</v>
       </c>
     </row>
-    <row r="156" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
         <v>307</v>
       </c>
@@ -5212,7 +5565,7 @@
         <v>3.1241996054094601E-2</v>
       </c>
     </row>
-    <row r="157" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
         <v>371</v>
       </c>
@@ -5229,7 +5582,7 @@
         <v>3.1241996054094601E-2</v>
       </c>
     </row>
-    <row r="158" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
         <v>405</v>
       </c>
@@ -5246,7 +5599,7 @@
         <v>3.1241996054094601E-2</v>
       </c>
     </row>
-    <row r="159" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
         <v>408</v>
       </c>
@@ -5263,7 +5616,7 @@
         <v>3.5603026257231898E-2</v>
       </c>
     </row>
-    <row r="160" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
         <v>346</v>
       </c>
@@ -5280,7 +5633,7 @@
         <v>3.0851637793439201E-2</v>
       </c>
     </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
         <v>90</v>
       </c>
@@ -5297,7 +5650,7 @@
         <v>2.65404589652047E-2</v>
       </c>
     </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
         <v>38</v>
       </c>
@@ -5314,7 +5667,7 @@
         <v>3.2636107402462498E-2</v>
       </c>
     </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
         <v>13</v>
       </c>
@@ -5331,7 +5684,7 @@
         <v>3.2227915820683899E-2</v>
       </c>
     </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
         <v>205</v>
       </c>
@@ -5348,7 +5701,7 @@
         <v>1.1584545312315399E-2</v>
       </c>
     </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
         <v>201</v>
       </c>
@@ -5365,7 +5718,7 @@
         <v>1.55138905197939E-2</v>
       </c>
     </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
         <v>383</v>
       </c>
@@ -5382,7 +5735,7 @@
         <v>1.55138905197939E-2</v>
       </c>
     </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
         <v>261</v>
       </c>
@@ -5399,7 +5752,7 @@
         <v>3.0054398461214799E-2</v>
       </c>
     </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
         <v>204</v>
       </c>
@@ -5416,7 +5769,7 @@
         <v>2.9669188547693199E-2</v>
       </c>
     </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
         <v>221</v>
       </c>
@@ -5433,7 +5786,7 @@
         <v>2.9669188547693199E-2</v>
       </c>
     </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
         <v>339</v>
       </c>
@@ -5450,7 +5803,7 @@
         <v>1.4466033913697E-2</v>
       </c>
     </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
         <v>417</v>
       </c>
@@ -5467,7 +5820,7 @@
         <v>1.39646745173758E-2</v>
       </c>
     </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
         <v>395</v>
       </c>
@@ -5484,7 +5837,7 @@
         <v>2.7048958615093301E-2</v>
       </c>
     </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
         <v>301</v>
       </c>
@@ -5501,7 +5854,7 @@
         <v>1.5416995720703401E-2</v>
       </c>
     </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
         <v>244</v>
       </c>
@@ -5518,7 +5871,7 @@
         <v>2.67022696929239E-2</v>
       </c>
     </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
         <v>506</v>
       </c>
@@ -5535,7 +5888,7 @@
         <v>2.67022696929239E-2</v>
       </c>
     </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
         <v>552</v>
       </c>
@@ -5552,7 +5905,7 @@
         <v>2.67022696929239E-2</v>
       </c>
     </row>
-    <row r="177" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
         <v>277</v>
       </c>
@@ -5569,7 +5922,7 @@
         <v>2.5782332656547099E-2</v>
       </c>
     </row>
-    <row r="178" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
         <v>517</v>
       </c>
@@ -5586,7 +5939,7 @@
         <v>2.5782332656547099E-2</v>
       </c>
     </row>
-    <row r="179" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
         <v>336</v>
       </c>
@@ -5603,7 +5956,7 @@
         <v>1.2411112415835099E-2</v>
       </c>
     </row>
-    <row r="180" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
         <v>291</v>
       </c>
@@ -5620,7 +5973,7 @@
         <v>1.0709412560710599E-2</v>
       </c>
     </row>
-    <row r="181" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
         <v>227</v>
       </c>
@@ -5637,7 +5990,7 @@
         <v>2.4043518768971799E-2</v>
       </c>
     </row>
-    <row r="182" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
         <v>135</v>
       </c>
@@ -5654,7 +6007,7 @@
         <v>1.9722705170197499E-2</v>
       </c>
     </row>
-    <row r="183" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
         <v>193</v>
       </c>
@@ -5671,7 +6024,7 @@
         <v>1.9359282653578301E-2</v>
       </c>
     </row>
-    <row r="184" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
         <v>85</v>
       </c>
@@ -5688,7 +6041,7 @@
         <v>1.29462644454894E-2</v>
       </c>
     </row>
-    <row r="185" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
         <v>363</v>
       </c>
@@ -5705,7 +6058,7 @@
         <v>1.29462644454894E-2</v>
       </c>
     </row>
-    <row r="186" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
         <v>105</v>
       </c>
@@ -5722,7 +6075,7 @@
         <v>1.9440734623280699E-2</v>
       </c>
     </row>
-    <row r="187" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
         <v>213</v>
       </c>
@@ -5739,7 +6092,7 @@
         <v>1.9440734623280699E-2</v>
       </c>
     </row>
-    <row r="188" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
         <v>241</v>
       </c>
@@ -5756,7 +6109,7 @@
         <v>1.9440734623280699E-2</v>
       </c>
     </row>
-    <row r="189" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
         <v>310</v>
       </c>
@@ -5773,7 +6126,7 @@
         <v>1.9440734623280699E-2</v>
       </c>
     </row>
-    <row r="190" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
         <v>234</v>
       </c>
@@ -5790,7 +6143,7 @@
         <v>2.37353508381546E-2</v>
       </c>
     </row>
-    <row r="191" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
         <v>267</v>
       </c>
@@ -5807,7 +6160,7 @@
         <v>2.37353508381546E-2</v>
       </c>
     </row>
-    <row r="192" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
         <v>376</v>
       </c>
@@ -5824,7 +6177,7 @@
         <v>2.37353508381546E-2</v>
       </c>
     </row>
-    <row r="193" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
         <v>404</v>
       </c>
@@ -5841,7 +6194,7 @@
         <v>2.37353508381546E-2</v>
       </c>
     </row>
-    <row r="194" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
         <v>420</v>
       </c>
@@ -5858,7 +6211,7 @@
         <v>2.37353508381546E-2</v>
       </c>
     </row>
-    <row r="195" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
         <v>386</v>
       </c>
@@ -5875,7 +6228,7 @@
         <v>1.8022960694123701E-2</v>
       </c>
     </row>
-    <row r="196" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
         <v>299</v>
       </c>
@@ -5892,7 +6245,7 @@
         <v>1.41156812942595E-2</v>
       </c>
     </row>
-    <row r="197" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
         <v>264</v>
       </c>
@@ -5909,7 +6262,7 @@
         <v>1.1430857509492401E-2</v>
       </c>
     </row>
-    <row r="198" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
         <v>400</v>
       </c>
@@ -5926,7 +6279,7 @@
         <v>2.1038078922850399E-2</v>
       </c>
     </row>
-    <row r="199" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
         <v>260</v>
       </c>
@@ -5943,7 +6296,7 @@
         <v>1.2923888752265401E-2</v>
       </c>
     </row>
-    <row r="200" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
         <v>65</v>
       </c>
@@ -5960,7 +6313,7 @@
         <v>2.0768431983385301E-2</v>
       </c>
     </row>
-    <row r="201" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
         <v>303</v>
       </c>
@@ -5977,7 +6330,7 @@
         <v>2.0768431983385301E-2</v>
       </c>
     </row>
-    <row r="202" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A202" t="s">
         <v>315</v>
       </c>
@@ -5994,7 +6347,7 @@
         <v>2.0768431983385301E-2</v>
       </c>
     </row>
-    <row r="203" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A203" t="s">
         <v>387</v>
       </c>
@@ -6011,7 +6364,7 @@
         <v>2.0768431983385301E-2</v>
       </c>
     </row>
-    <row r="204" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A204" t="s">
         <v>448</v>
       </c>
@@ -6028,7 +6381,7 @@
         <v>2.0768431983385301E-2</v>
       </c>
     </row>
-    <row r="205" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A205" t="s">
         <v>462</v>
       </c>
@@ -6045,7 +6398,7 @@
         <v>2.0768431983385301E-2</v>
       </c>
     </row>
-    <row r="206" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A206" t="s">
         <v>73</v>
       </c>
@@ -6062,7 +6415,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="207" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A207" t="s">
         <v>130</v>
       </c>
@@ -6079,7 +6432,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="208" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A208" t="s">
         <v>292</v>
       </c>
@@ -6096,7 +6449,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="209" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A209" t="s">
         <v>465</v>
       </c>
@@ -6113,7 +6466,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="210" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A210" t="s">
         <v>481</v>
       </c>
@@ -6130,7 +6483,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="211" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A211" t="s">
         <v>485</v>
       </c>
@@ -6147,7 +6500,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="212" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A212" t="s">
         <v>514</v>
       </c>
@@ -6164,7 +6517,7 @@
         <v>1.93367494924103E-2</v>
       </c>
     </row>
-    <row r="213" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A213" t="s">
         <v>189</v>
       </c>
@@ -6181,7 +6534,7 @@
         <v>5.1291920260954603E-3</v>
       </c>
     </row>
-    <row r="214" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A214" t="s">
         <v>23</v>
       </c>
@@ -6198,7 +6551,7 @@
         <v>1.3514539108010299E-2</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A215" t="s">
         <v>98</v>
       </c>
@@ -6215,7 +6568,7 @@
         <v>1.3514539108010299E-2</v>
       </c>
     </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A216" t="s">
         <v>317</v>
       </c>
@@ -6232,7 +6585,7 @@
         <v>1.3514539108010299E-2</v>
       </c>
     </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A217" t="s">
         <v>351</v>
       </c>
@@ -6249,7 +6602,7 @@
         <v>1.3514539108010299E-2</v>
       </c>
     </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A218" t="s">
         <v>498</v>
       </c>
@@ -6266,7 +6619,7 @@
         <v>1.3514539108010299E-2</v>
       </c>
     </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A219" t="s">
         <v>432</v>
       </c>
@@ -6283,7 +6636,7 @@
         <v>8.9590970593005793E-3</v>
       </c>
     </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A220" t="s">
         <v>242</v>
       </c>
@@ -6300,7 +6653,7 @@
         <v>1.3583570046443399E-2</v>
       </c>
     </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A221" t="s">
         <v>401</v>
       </c>
@@ -6317,7 +6670,7 @@
         <v>1.7801513128615901E-2</v>
       </c>
     </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A222" t="s">
         <v>515</v>
       </c>
@@ -6334,7 +6687,7 @@
         <v>1.7801513128615901E-2</v>
       </c>
     </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A223" t="s">
         <v>323</v>
       </c>
@@ -6351,7 +6704,7 @@
         <v>1.6113957910341901E-2</v>
       </c>
     </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A224" t="s">
         <v>392</v>
       </c>
@@ -6368,7 +6721,7 @@
         <v>1.1693491025124901E-2</v>
       </c>
     </row>
-    <row r="225" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A225" t="s">
         <v>15</v>
       </c>
@@ -6385,7 +6738,7 @@
         <v>8.0451303858133007E-3</v>
       </c>
     </row>
-    <row r="226" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A226" t="s">
         <v>185</v>
       </c>
@@ -6402,7 +6755,7 @@
         <v>7.9623139277405705E-3</v>
       </c>
     </row>
-    <row r="227" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A227" t="s">
         <v>427</v>
       </c>
@@ -6419,7 +6772,7 @@
         <v>5.7897015175390103E-3</v>
       </c>
     </row>
-    <row r="228" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A228" t="s">
         <v>72</v>
       </c>
@@ -6436,7 +6789,7 @@
         <v>1.5027199230607399E-2</v>
       </c>
     </row>
-    <row r="229" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A229" t="s">
         <v>285</v>
       </c>
@@ -6453,7 +6806,7 @@
         <v>1.5027199230607399E-2</v>
       </c>
     </row>
-    <row r="230" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A230" t="s">
         <v>356</v>
       </c>
@@ -6470,7 +6823,7 @@
         <v>1.0847014409685701E-2</v>
       </c>
     </row>
-    <row r="231" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A231" t="s">
         <v>159</v>
       </c>
@@ -6487,7 +6840,7 @@
         <v>1.06867583455365E-2</v>
       </c>
     </row>
-    <row r="232" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A232" t="s">
         <v>206</v>
       </c>
@@ -6504,7 +6857,7 @@
         <v>1.06867583455365E-2</v>
       </c>
     </row>
-    <row r="233" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A233" t="s">
         <v>327</v>
       </c>
@@ -6521,7 +6874,7 @@
         <v>1.06867583455365E-2</v>
       </c>
     </row>
-    <row r="234" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A234" t="s">
         <v>126</v>
       </c>
@@ -6538,7 +6891,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="235" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A235" t="s">
         <v>176</v>
       </c>
@@ -6555,7 +6908,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="236" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A236" t="s">
         <v>349</v>
       </c>
@@ -6572,7 +6925,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="237" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A237" t="s">
         <v>380</v>
       </c>
@@ -6589,7 +6942,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="238" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A238" t="s">
         <v>416</v>
       </c>
@@ -6606,7 +6959,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="239" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A239" t="s">
         <v>489</v>
       </c>
@@ -6623,7 +6976,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="240" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A240" t="s">
         <v>505</v>
       </c>
@@ -6640,7 +6993,7 @@
         <v>1.4834594273846599E-2</v>
       </c>
     </row>
-    <row r="241" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A241" t="s">
         <v>215</v>
       </c>
@@ -6657,7 +7010,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="242" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A242" t="s">
         <v>374</v>
       </c>
@@ -6674,7 +7027,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="243" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A243" t="s">
         <v>393</v>
       </c>
@@ -6691,7 +7044,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="244" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A244" t="s">
         <v>439</v>
       </c>
@@ -6708,7 +7061,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="245" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A245" t="s">
         <v>469</v>
       </c>
@@ -6725,7 +7078,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="246" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A246" t="s">
         <v>480</v>
       </c>
@@ -6742,7 +7095,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="247" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A247" t="s">
         <v>518</v>
       </c>
@@ -6759,7 +7112,7 @@
         <v>1.2891166328273499E-2</v>
       </c>
     </row>
-    <row r="248" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A248" t="s">
         <v>240</v>
       </c>
@@ -6776,7 +7129,7 @@
         <v>6.2055562079175496E-3</v>
       </c>
     </row>
-    <row r="249" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A249" t="s">
         <v>454</v>
       </c>
@@ -6793,7 +7146,7 @@
         <v>6.2055562079175496E-3</v>
       </c>
     </row>
-    <row r="250" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A250" t="s">
         <v>19</v>
       </c>
@@ -6810,7 +7163,7 @@
         <v>7.9134496201001703E-3</v>
       </c>
     </row>
-    <row r="251" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A251" t="s">
         <v>460</v>
       </c>
@@ -6827,7 +7180,7 @@
         <v>2.82599778209899E-3</v>
       </c>
     </row>
-    <row r="252" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A252" t="s">
         <v>397</v>
       </c>
@@ -6844,7 +7197,7 @@
         <v>7.8054192500486798E-3</v>
       </c>
     </row>
-    <row r="253" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A253" t="s">
         <v>128</v>
       </c>
@@ -6861,7 +7214,7 @@
         <v>1.20217593844859E-2</v>
       </c>
     </row>
-    <row r="254" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A254" t="s">
         <v>248</v>
       </c>
@@ -6878,7 +7231,7 @@
         <v>1.20217593844859E-2</v>
       </c>
     </row>
-    <row r="255" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A255" t="s">
         <v>116</v>
       </c>
@@ -6895,7 +7248,7 @@
         <v>7.8425408922572805E-3</v>
       </c>
     </row>
-    <row r="256" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A256" t="s">
         <v>255</v>
       </c>
@@ -6912,7 +7265,7 @@
         <v>7.8425408922572805E-3</v>
       </c>
     </row>
-    <row r="257" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A257" t="s">
         <v>300</v>
       </c>
@@ -6929,7 +7282,7 @@
         <v>7.8425408922572805E-3</v>
       </c>
     </row>
-    <row r="258" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A258" t="s">
         <v>200</v>
       </c>
@@ -6946,7 +7299,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="259" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
         <v>256</v>
       </c>
@@ -6963,7 +7316,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="260" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A260" t="s">
         <v>325</v>
       </c>
@@ -6980,7 +7333,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="261" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A261" t="s">
         <v>334</v>
       </c>
@@ -6997,7 +7350,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="262" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A262" t="s">
         <v>348</v>
       </c>
@@ -7014,7 +7367,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="263" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A263" t="s">
         <v>362</v>
       </c>
@@ -7031,7 +7384,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="264" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A264" t="s">
         <v>433</v>
       </c>
@@ -7048,7 +7401,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="265" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A265" t="s">
         <v>438</v>
       </c>
@@ -7065,7 +7418,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="266" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A266" t="s">
         <v>455</v>
       </c>
@@ -7082,7 +7435,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="267" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A267" t="s">
         <v>474</v>
       </c>
@@ -7099,7 +7452,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="268" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A268" t="s">
         <v>493</v>
       </c>
@@ -7116,7 +7469,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="269" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A269" t="s">
         <v>502</v>
       </c>
@@ -7133,7 +7486,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="270" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A270" t="s">
         <v>525</v>
       </c>
@@ -7150,7 +7503,7 @@
         <v>1.18676754190773E-2</v>
       </c>
     </row>
-    <row r="271" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A271" t="s">
         <v>364</v>
       </c>
@@ -7167,7 +7520,7 @@
         <v>9.6683747462051606E-3</v>
       </c>
     </row>
-    <row r="272" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A272" t="s">
         <v>407</v>
       </c>
@@ -7184,7 +7537,7 @@
         <v>9.6683747462051606E-3</v>
       </c>
     </row>
-    <row r="273" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A273" t="s">
         <v>496</v>
       </c>
@@ -7201,7 +7554,7 @@
         <v>9.6683747462051606E-3</v>
       </c>
     </row>
-    <row r="274" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A274" t="s">
         <v>294</v>
       </c>
@@ -7218,7 +7571,7 @@
         <v>5.5879001062051998E-3</v>
       </c>
     </row>
-    <row r="275" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A275" t="s">
         <v>367</v>
       </c>
@@ -7235,7 +7588,7 @@
         <v>5.5879001062051998E-3</v>
       </c>
     </row>
-    <row r="276" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A276" t="s">
         <v>527</v>
       </c>
@@ -7252,7 +7605,7 @@
         <v>5.5879001062051998E-3</v>
       </c>
     </row>
-    <row r="277" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A277" t="s">
         <v>162</v>
       </c>
@@ -7269,7 +7622,7 @@
         <v>5.2101101507629598E-3</v>
       </c>
     </row>
-    <row r="278" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A278" t="s">
         <v>129</v>
       </c>
@@ -7286,7 +7639,7 @@
         <v>9.0163195383644399E-3</v>
       </c>
     </row>
-    <row r="279" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A279" t="s">
         <v>133</v>
       </c>
@@ -7303,7 +7656,7 @@
         <v>9.0163195383644399E-3</v>
       </c>
     </row>
-    <row r="280" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A280" t="s">
         <v>237</v>
       </c>
@@ -7320,7 +7673,7 @@
         <v>9.0163195383644399E-3</v>
       </c>
     </row>
-    <row r="281" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A281" t="s">
         <v>275</v>
       </c>
@@ -7337,7 +7690,7 @@
         <v>5.1389985735677997E-3</v>
       </c>
     </row>
-    <row r="282" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A282" t="s">
         <v>41</v>
       </c>
@@ -7354,7 +7707,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="283" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A283" t="s">
         <v>216</v>
       </c>
@@ -7371,7 +7724,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="284" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A284" t="s">
         <v>316</v>
       </c>
@@ -7388,7 +7741,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="285" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A285" t="s">
         <v>388</v>
       </c>
@@ -7405,7 +7758,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="286" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A286" t="s">
         <v>398</v>
       </c>
@@ -7422,7 +7775,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="287" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A287" t="s">
         <v>424</v>
       </c>
@@ -7439,7 +7792,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="288" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A288" t="s">
         <v>430</v>
       </c>
@@ -7456,7 +7809,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="289" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A289" t="s">
         <v>434</v>
       </c>
@@ -7473,7 +7826,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="290" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A290" t="s">
         <v>436</v>
       </c>
@@ -7490,7 +7843,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="291" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A291" t="s">
         <v>458</v>
       </c>
@@ -7507,7 +7860,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="292" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A292" t="s">
         <v>487</v>
       </c>
@@ -7524,7 +7877,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="293" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A293" t="s">
         <v>491</v>
       </c>
@@ -7541,7 +7894,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="294" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A294" t="s">
         <v>512</v>
       </c>
@@ -7558,7 +7911,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="295" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A295" t="s">
         <v>544</v>
       </c>
@@ -7575,7 +7928,7 @@
         <v>8.9007565643079694E-3</v>
       </c>
     </row>
-    <row r="296" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A296" t="s">
         <v>31</v>
       </c>
@@ -7592,7 +7945,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="297" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A297" t="s">
         <v>137</v>
       </c>
@@ -7609,7 +7962,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="298" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A298" t="s">
         <v>140</v>
       </c>
@@ -7626,7 +7979,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="299" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A299" t="s">
         <v>160</v>
       </c>
@@ -7643,7 +7996,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="300" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A300" t="s">
         <v>251</v>
       </c>
@@ -7660,7 +8013,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="301" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A301" t="s">
         <v>343</v>
       </c>
@@ -7677,7 +8030,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="302" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A302" t="s">
         <v>366</v>
       </c>
@@ -7694,7 +8047,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="303" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A303" t="s">
         <v>418</v>
       </c>
@@ -7711,7 +8064,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="304" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A304" t="s">
         <v>478</v>
       </c>
@@ -7728,7 +8081,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="305" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A305" t="s">
         <v>482</v>
       </c>
@@ -7745,7 +8098,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="306" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A306" t="s">
         <v>523</v>
       </c>
@@ -7762,7 +8115,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="307" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A307" t="s">
         <v>534</v>
       </c>
@@ -7779,7 +8132,7 @@
         <v>6.4455831641367697E-3</v>
       </c>
     </row>
-    <row r="308" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A308" t="s">
         <v>311</v>
       </c>
@@ -7796,7 +8149,7 @@
         <v>3.1197993547041401E-3</v>
       </c>
     </row>
-    <row r="309" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A309" t="s">
         <v>524</v>
       </c>
@@ -7813,7 +8166,7 @@
         <v>3.1197993547041401E-3</v>
       </c>
     </row>
-    <row r="310" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="310" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A310" t="s">
         <v>199</v>
       </c>
@@ -7830,7 +8183,7 @@
         <v>3.10277810395878E-3</v>
       </c>
     </row>
-    <row r="311" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="311" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A311" t="s">
         <v>389</v>
       </c>
@@ -7847,7 +8200,7 @@
         <v>3.10277810395878E-3</v>
       </c>
     </row>
-    <row r="312" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="312" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A312" t="s">
         <v>62</v>
       </c>
@@ -7864,7 +8217,7 @@
         <v>6.0108796922429602E-3</v>
       </c>
     </row>
-    <row r="313" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="313" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A313" t="s">
         <v>360</v>
       </c>
@@ -7881,7 +8234,7 @@
         <v>6.0108796922429602E-3</v>
       </c>
     </row>
-    <row r="314" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="314" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A314" t="s">
         <v>406</v>
       </c>
@@ -7898,7 +8251,7 @@
         <v>6.0108796922429602E-3</v>
       </c>
     </row>
-    <row r="315" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="315" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A315" t="s">
         <v>440</v>
       </c>
@@ -7915,7 +8268,7 @@
         <v>6.0108796922429602E-3</v>
       </c>
     </row>
-    <row r="316" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="316" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A316" t="s">
         <v>459</v>
       </c>
@@ -7932,7 +8285,7 @@
         <v>6.0108796922429602E-3</v>
       </c>
     </row>
-    <row r="317" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="317" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A317" t="s">
         <v>495</v>
       </c>
@@ -7949,7 +8302,7 @@
         <v>6.0108796922429602E-3</v>
       </c>
     </row>
-    <row r="318" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="318" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A318" t="s">
         <v>340</v>
       </c>
@@ -7966,7 +8319,7 @@
         <v>2.9863656864335302E-3</v>
       </c>
     </row>
-    <row r="319" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="319" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A319" t="s">
         <v>385</v>
       </c>
@@ -7983,7 +8336,7 @@
         <v>2.9863656864335302E-3</v>
       </c>
     </row>
-    <row r="320" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="320" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A320" t="s">
         <v>409</v>
       </c>
@@ -8000,7 +8353,7 @@
         <v>2.9863656864335302E-3</v>
       </c>
     </row>
-    <row r="321" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="321" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A321" t="s">
         <v>452</v>
       </c>
@@ -8017,7 +8370,7 @@
         <v>2.9863656864335302E-3</v>
       </c>
     </row>
-    <row r="322" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="322" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A322" t="s">
         <v>78</v>
       </c>
@@ -8034,7 +8387,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="323" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="323" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A323" t="s">
         <v>168</v>
       </c>
@@ -8051,7 +8404,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="324" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="324" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A324" t="s">
         <v>223</v>
       </c>
@@ -8068,7 +8421,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="325" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="325" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A325" t="s">
         <v>274</v>
       </c>
@@ -8085,7 +8438,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="326" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="326" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A326" t="s">
         <v>286</v>
       </c>
@@ -8102,7 +8455,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="327" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="327" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A327" t="s">
         <v>287</v>
       </c>
@@ -8119,7 +8472,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="328" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="328" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A328" t="s">
         <v>288</v>
       </c>
@@ -8136,7 +8489,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="329" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="329" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A329" t="s">
         <v>320</v>
       </c>
@@ -8153,7 +8506,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="330" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="330" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A330" t="s">
         <v>322</v>
       </c>
@@ -8170,7 +8523,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="331" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="331" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A331" t="s">
         <v>330</v>
       </c>
@@ -8187,7 +8540,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="332" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="332" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A332" t="s">
         <v>333</v>
       </c>
@@ -8204,7 +8557,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="333" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="333" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A333" t="s">
         <v>345</v>
       </c>
@@ -8221,7 +8574,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="334" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="334" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A334" t="s">
         <v>372</v>
       </c>
@@ -8238,7 +8591,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="335" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="335" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A335" t="s">
         <v>414</v>
       </c>
@@ -8255,7 +8608,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="336" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="336" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A336" t="s">
         <v>422</v>
       </c>
@@ -8272,7 +8625,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="337" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="337" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A337" t="s">
         <v>425</v>
       </c>
@@ -8289,7 +8642,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="338" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="338" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A338" t="s">
         <v>447</v>
       </c>
@@ -8306,7 +8659,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="339" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="339" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A339" t="s">
         <v>451</v>
       </c>
@@ -8323,7 +8676,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="340" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="340" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A340" t="s">
         <v>488</v>
       </c>
@@ -8340,7 +8693,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="341" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="341" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A341" t="s">
         <v>519</v>
       </c>
@@ -8357,7 +8710,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="342" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="342" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A342" t="s">
         <v>522</v>
       </c>
@@ -8374,7 +8727,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="343" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="343" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A343" t="s">
         <v>538</v>
       </c>
@@ -8391,7 +8744,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="344" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="344" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A344" t="s">
         <v>540</v>
       </c>
@@ -8408,7 +8761,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="345" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="345" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A345" t="s">
         <v>541</v>
       </c>
@@ -8425,7 +8778,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="346" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="346" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A346" t="s">
         <v>543</v>
       </c>
@@ -8442,7 +8795,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="347" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="347" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A347" t="s">
         <v>553</v>
       </c>
@@ -8459,7 +8812,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="348" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="348" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A348" t="s">
         <v>555</v>
       </c>
@@ -8476,7 +8829,7 @@
         <v>5.9338377095386396E-3</v>
       </c>
     </row>
-    <row r="349" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="349" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A349" t="s">
         <v>95</v>
       </c>
@@ -8493,7 +8846,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="350" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="350" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A350" t="s">
         <v>106</v>
       </c>
@@ -8510,7 +8863,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="351" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="351" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A351" t="s">
         <v>123</v>
       </c>
@@ -8527,7 +8880,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="352" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="352" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A352" t="s">
         <v>165</v>
       </c>
@@ -8544,7 +8897,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="353" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="353" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A353" t="s">
         <v>238</v>
       </c>
@@ -8561,7 +8914,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="354" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="354" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A354" t="s">
         <v>257</v>
       </c>
@@ -8578,7 +8931,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="355" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="355" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A355" t="s">
         <v>270</v>
       </c>
@@ -8595,7 +8948,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="356" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="356" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A356" t="s">
         <v>271</v>
       </c>
@@ -8612,7 +8965,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="357" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="357" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A357" t="s">
         <v>359</v>
       </c>
@@ -8629,7 +8982,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="358" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="358" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A358" t="s">
         <v>442</v>
       </c>
@@ -8646,7 +8999,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="359" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="359" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A359" t="s">
         <v>444</v>
       </c>
@@ -8663,7 +9016,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="360" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="360" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A360" t="s">
         <v>457</v>
       </c>
@@ -8680,7 +9033,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="361" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="361" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A361" t="s">
         <v>464</v>
       </c>
@@ -8697,7 +9050,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="362" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="362" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A362" t="s">
         <v>492</v>
       </c>
@@ -8714,7 +9067,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="363" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="363" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A363" t="s">
         <v>503</v>
       </c>
@@ -8731,7 +9084,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="364" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="364" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A364" t="s">
         <v>508</v>
       </c>
@@ -8748,7 +9101,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="365" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="365" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A365" t="s">
         <v>533</v>
       </c>
@@ -8765,7 +9118,7 @@
         <v>3.22279158206839E-3</v>
       </c>
     </row>
-    <row r="366" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="366" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A366" t="s">
         <v>39</v>
       </c>
@@ -8782,7 +9135,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="367" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="367" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A367" t="s">
         <v>132</v>
       </c>
@@ -8799,7 +9152,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="368" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="368" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A368" t="s">
         <v>155</v>
       </c>
@@ -8816,7 +9169,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="369" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="369" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A369" t="s">
         <v>157</v>
       </c>
@@ -8833,7 +9186,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="370" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="370" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A370" t="s">
         <v>232</v>
       </c>
@@ -8850,7 +9203,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="371" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="371" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A371" t="s">
         <v>262</v>
       </c>
@@ -8867,7 +9220,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="372" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="372" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A372" t="s">
         <v>273</v>
       </c>
@@ -8884,7 +9237,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="373" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="373" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A373" t="s">
         <v>278</v>
       </c>
@@ -8901,7 +9254,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="374" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="374" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A374" t="s">
         <v>290</v>
       </c>
@@ -8918,7 +9271,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="375" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="375" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A375" t="s">
         <v>297</v>
       </c>
@@ -8935,7 +9288,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="376" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A376" t="s">
         <v>304</v>
       </c>
@@ -8952,7 +9305,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="377" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="377" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A377" t="s">
         <v>321</v>
       </c>
@@ -8969,7 +9322,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="378" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="378" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A378" t="s">
         <v>341</v>
       </c>
@@ -8986,7 +9339,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="379" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="379" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A379" t="s">
         <v>352</v>
       </c>
@@ -9003,7 +9356,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="380" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="380" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A380" t="s">
         <v>354</v>
       </c>
@@ -9020,7 +9373,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="381" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="381" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A381" t="s">
         <v>357</v>
       </c>
@@ -9037,7 +9390,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="382" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="382" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A382" t="s">
         <v>399</v>
       </c>
@@ -9054,7 +9407,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="383" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="383" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A383" t="s">
         <v>419</v>
       </c>
@@ -9071,7 +9424,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="384" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="384" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A384" t="s">
         <v>450</v>
       </c>
@@ -9088,7 +9441,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="385" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="385" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A385" t="s">
         <v>467</v>
       </c>
@@ -9105,7 +9458,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="386" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="386" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A386" t="s">
         <v>472</v>
       </c>
@@ -9122,7 +9475,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="387" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="387" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A387" t="s">
         <v>529</v>
       </c>
@@ -9139,7 +9492,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="388" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="388" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A388" t="s">
         <v>532</v>
       </c>
@@ -9156,7 +9509,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="389" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="389" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A389" t="s">
         <v>550</v>
       </c>
@@ -9173,7 +9526,7 @@
         <v>3.0054398461214801E-3</v>
       </c>
     </row>
-    <row r="390" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="390" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A390" t="s">
         <v>24</v>
       </c>
@@ -9190,7 +9543,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="391" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="391" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
         <v>49</v>
       </c>
@@ -9207,7 +9560,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="392" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="392" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A392" t="s">
         <v>68</v>
       </c>
@@ -9224,7 +9577,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="393" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="393" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A393" t="s">
         <v>118</v>
       </c>
@@ -9241,7 +9594,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="394" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="394" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A394" t="s">
         <v>125</v>
       </c>
@@ -9258,7 +9611,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="395" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="395" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A395" t="s">
         <v>172</v>
       </c>
@@ -9275,7 +9628,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="396" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="396" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A396" t="s">
         <v>293</v>
       </c>
@@ -9292,7 +9645,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="397" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="397" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A397" t="s">
         <v>305</v>
       </c>
@@ -9309,7 +9662,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="398" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="398" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A398" t="s">
         <v>308</v>
       </c>
@@ -9326,7 +9679,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="399" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="399" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A399" t="s">
         <v>326</v>
       </c>
@@ -9343,7 +9696,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="400" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="400" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A400" t="s">
         <v>350</v>
       </c>
@@ -9360,7 +9713,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="401" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="401" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A401" t="s">
         <v>353</v>
       </c>
@@ -9377,7 +9730,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="402" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="402" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A402" t="s">
         <v>365</v>
       </c>
@@ -9394,7 +9747,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="403" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="403" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A403" t="s">
         <v>368</v>
       </c>
@@ -9411,7 +9764,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="404" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="404" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A404" t="s">
         <v>379</v>
       </c>
@@ -9428,7 +9781,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="405" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="405" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A405" t="s">
         <v>384</v>
       </c>
@@ -9445,7 +9798,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="406" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="406" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A406" t="s">
         <v>394</v>
       </c>
@@ -9462,7 +9815,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="407" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="407" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A407" t="s">
         <v>396</v>
       </c>
@@ -9479,7 +9832,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="408" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="408" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A408" t="s">
         <v>402</v>
       </c>
@@ -9496,7 +9849,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="409" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="409" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A409" t="s">
         <v>412</v>
       </c>
@@ -9513,7 +9866,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="410" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="410" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A410" t="s">
         <v>415</v>
       </c>
@@ -9530,7 +9883,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="411" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="411" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A411" t="s">
         <v>429</v>
       </c>
@@ -9547,7 +9900,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="412" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="412" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A412" t="s">
         <v>431</v>
       </c>
@@ -9564,7 +9917,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="413" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="413" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A413" t="s">
         <v>435</v>
       </c>
@@ -9581,7 +9934,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="414" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="414" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A414" t="s">
         <v>443</v>
       </c>
@@ -9598,7 +9951,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="415" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="415" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A415" t="s">
         <v>445</v>
       </c>
@@ -9615,7 +9968,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="416" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="416" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A416" t="s">
         <v>453</v>
       </c>
@@ -9632,7 +9985,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="417" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="417" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A417" t="s">
         <v>456</v>
       </c>
@@ -9649,7 +10002,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="418" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="418" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A418" t="s">
         <v>461</v>
       </c>
@@ -9666,7 +10019,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="419" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="419" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A419" t="s">
         <v>463</v>
       </c>
@@ -9683,7 +10036,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="420" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="420" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A420" t="s">
         <v>468</v>
       </c>
@@ -9700,7 +10053,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="421" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="421" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A421" t="s">
         <v>470</v>
       </c>
@@ -9717,7 +10070,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="422" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="422" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A422" t="s">
         <v>473</v>
       </c>
@@ -9734,7 +10087,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="423" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="423" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A423" t="s">
         <v>476</v>
       </c>
@@ -9751,7 +10104,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="424" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="424" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A424" t="s">
         <v>477</v>
       </c>
@@ -9768,7 +10121,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="425" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="425" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A425" t="s">
         <v>483</v>
       </c>
@@ -9785,7 +10138,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="426" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="426" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A426" t="s">
         <v>490</v>
       </c>
@@ -9802,7 +10155,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="427" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="427" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A427" t="s">
         <v>494</v>
       </c>
@@ -9819,7 +10172,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="428" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="428" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A428" t="s">
         <v>500</v>
       </c>
@@ -9836,7 +10189,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="429" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="429" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A429" t="s">
         <v>501</v>
       </c>
@@ -9853,7 +10206,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="430" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="430" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A430" t="s">
         <v>509</v>
       </c>
@@ -9870,7 +10223,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="431" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="431" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A431" t="s">
         <v>510</v>
       </c>
@@ -9887,7 +10240,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="432" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="432" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A432" t="s">
         <v>511</v>
       </c>
@@ -9904,7 +10257,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="433" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="433" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A433" t="s">
         <v>516</v>
       </c>
@@ -9921,7 +10274,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="434" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="434" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A434" t="s">
         <v>521</v>
       </c>
@@ -9938,7 +10291,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="435" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="435" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A435" t="s">
         <v>528</v>
       </c>
@@ -9955,7 +10308,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="436" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="436" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A436" t="s">
         <v>530</v>
       </c>
@@ -9972,7 +10325,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="437" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="437" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A437" t="s">
         <v>535</v>
       </c>
@@ -9989,7 +10342,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="438" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="438" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A438" t="s">
         <v>536</v>
       </c>
@@ -10006,7 +10359,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="439" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="439" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A439" t="s">
         <v>537</v>
       </c>
@@ -10023,7 +10376,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="440" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="440" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A440" t="s">
         <v>539</v>
       </c>
@@ -10040,7 +10393,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="441" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="441" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A441" t="s">
         <v>542</v>
       </c>
@@ -10057,7 +10410,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="442" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="442" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A442" t="s">
         <v>546</v>
       </c>
@@ -10074,7 +10427,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="443" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="443" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A443" t="s">
         <v>548</v>
       </c>
@@ -10091,7 +10444,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="444" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="444" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A444" t="s">
         <v>549</v>
       </c>
@@ -10108,7 +10461,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="445" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="445" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A445" t="s">
         <v>554</v>
       </c>
@@ -10125,7 +10478,7 @@
         <v>2.9669188547693198E-3</v>
       </c>
     </row>
-    <row r="446" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="446" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A446" t="s">
         <v>556</v>
       </c>

</xml_diff>